<commit_message>
Update Antall og andel sysselsatte i Vestfold 2023 SSB 07984 06445.xlsx
oppdateringer
</commit_message>
<xml_diff>
--- a/03_Arbeid og næringsliv/Sysselsetting/2022/Antall og andel sysselsatte i Vestfold 2023 SSB 07984 06445.xlsx
+++ b/03_Arbeid og næringsliv/Sysselsetting/2022/Antall og andel sysselsatte i Vestfold 2023 SSB 07984 06445.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vestfoldfylke-my.sharepoint.com/personal/ellen_just_hansen_vestfoldfylke_no/Documents/Dokumenter/GitHub/Github-Kunnskap-om-Vestfold/Vestfold/03_Arbeid og næringsliv/Sysselsetting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vestfoldfylke-my.sharepoint.com/personal/ellen_just_hansen_vestfoldfylke_no/Documents/Dokumenter/GitHub/Nyeste Github versjon/Vestfold/03_Arbeid og næringsliv/Sysselsetting/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DF50362-A0F4-46BF-86D3-D802ECF446BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{0DF50362-A0F4-46BF-86D3-D802ECF446BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84A59610-9CE9-4BEC-A5BC-0290951123CF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,12 +520,14 @@
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="4" width="9.1796875" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">

</xml_diff>